<commit_message>
math checks: locate differences between 2016 script and manual computation
</commit_message>
<xml_diff>
--- a/documentation/variables.xlsx
+++ b/documentation/variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -153,11 +153,6 @@
 Estimate!!Percent with a disability!!Subject!!Total civilian noninstitutionalized population</t>
   </si>
   <si>
-    <t>S0101_C01_030
-AGE AND SEX
-Estimate!!Total!!Total population!!SELECTED AGE CATEGORIES!!65 years and over</t>
-  </si>
-  <si>
     <t>S0101_C02_030
 AGE AND SEX
 Estimate!!Percent!!Total population!!SELECTED AGE CATEGORIES!!65 years and over</t>
@@ -223,6 +218,11 @@
     <t>DP05_0003PE
 ACS DEMOGRAPHIC AND HOUSING ESTIMATES
 Percent Estimate!!SEX AND AGE!!Total population!!Female</t>
+  </si>
+  <si>
+    <t>DP05_0029E
+ACS DEMOGRAPHIC AND HOUSING ESTIMATES
+ Estimate!!SEX AND AGE!!Total population!!65 years and over</t>
   </si>
 </sst>
 </file>
@@ -258,13 +258,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -572,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,39 +592,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -667,7 +670,7 @@
         <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -698,22 +701,22 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -724,19 +727,19 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -747,13 +750,13 @@
         <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>33</v>
@@ -770,13 +773,13 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
         <v>33</v>
@@ -793,13 +796,13 @@
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
         <v>33</v>
@@ -816,13 +819,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>

</xml_diff>